<commit_message>
Feature ensembled with top 10 feature ranks
</commit_message>
<xml_diff>
--- a/NSL KDD/FeatureSelectionBinary/feature_ranking/chi2/chi_square_results_v2.xlsx
+++ b/NSL KDD/FeatureSelectionBinary/feature_ranking/chi2/chi_square_results_v2.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aravind/Projects/IntrusionDetection/IntrusionDetection/NSL KDD/FeatureSelectionBinary/feature_ranking/chi2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A682A76-05F3-FC45-B7FA-8A6E8EBA2715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -151,8 +170,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,13 +234,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -259,7 +286,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -293,6 +320,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -327,9 +355,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -502,14 +531,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -525,7 +560,7 @@
         <v>3340257591.445745</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -533,23 +568,23 @@
         <v>1746063122.170224</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>7082565.303892097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>7082565.3038920974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6968826.69801921</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>6968826.6980192102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -557,15 +592,15 @@
         <v>6525616.721263824</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>957425.8043037683</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>957425.80430376832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -573,23 +608,23 @@
         <v>82437.93955815387</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>54653.93292607195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>54653.932926071953</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>38543.82224319602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>38543.822243196017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -597,7 +632,7 @@
         <v>37451.32465887905</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -605,15 +640,15 @@
         <v>37364.83553764291</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>37225.46649294985</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>37225.466492949847</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -621,79 +656,79 @@
         <v>36259.73858447517</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>32550.97103273541</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>32550.971032735411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>26894.75327950227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>26894.753279502271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>23448.2085387342</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>23448.208538734201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>20826.41409626877</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>20826.414096268771</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>6997.367717676969</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>6997.3677176769688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>6923.373013273987</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>6923.3730132739875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>6866.941117392023</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>6866.9411173920234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>6354.755807978947</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>6354.7558079789469</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>4889.745829142064</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>4889.7458291420644</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -701,15 +736,15 @@
         <v>3282.67842401501</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>3197.842615103494</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>3197.8426151034942</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -717,15 +752,15 @@
         <v>2694.210071542976</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
-        <v>1723.289569546626</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>1723.2895695466259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -733,7 +768,7 @@
         <v>1245.395262157833</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -741,71 +776,71 @@
         <v>1053.573988677671</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
-        <v>692.7567558492688</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>692.75675584926876</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
-        <v>487.6709925760863</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>487.67099257608629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
-        <v>409.0339656797477</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>409.03396567974772</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
-        <v>192.5319501544994</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>192.53195015449941</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
-        <v>190.5539101395185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>190.55391013951851</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
-        <v>117.3052955440262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>117.30529554402619</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
-        <v>51.7693680244827</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>51.769368024482702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
-        <v>14.13591775299517</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>14.135917752995169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -813,39 +848,39 @@
         <v>13.47133902938325</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
-        <v>6.512199407543797</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>6.5121994075437968</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
-        <v>2.974008944179703</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>2.9740089441797029</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
-        <v>1.8171812299381</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>1.8171812299381001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.8706305129042797</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>0.87063051290427973</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>

</xml_diff>